<commit_message>
Added links to parts and prices in BOM
</commit_message>
<xml_diff>
--- a/AnalogComparator/Project Outputs for AnalogComparator/BOM/Bill of Materials-AnalogComparator.xlsx
+++ b/AnalogComparator/Project Outputs for AnalogComparator/BOM/Bill of Materials-AnalogComparator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\AnalogComparator\Project Outputs for AnalogComparator\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naomi_12/AnalogComparator/AnalogComparator/Project Outputs for AnalogComparator/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD03F8AA-06CD-4977-AA96-4245A20D73DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B512FB0-39B3-104B-ACAF-25285ECB82D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="19200" windowHeight="10010" xr2:uid="{472F2DBD-E0F5-4488-8DC5-87C56A307CF0}"/>
+    <workbookView xWindow="-300" yWindow="2120" windowWidth="23200" windowHeight="10020" xr2:uid="{472F2DBD-E0F5-4488-8DC5-87C56A307CF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-AnalogCompara" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="80">
   <si>
     <t>Comment</t>
   </si>
@@ -45,9 +45,6 @@
     <t>LibRef</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
     <t>47uF</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
     <t>CMP-2000-06898-1</t>
   </si>
   <si>
-    <t>73391-0083</t>
-  </si>
-  <si>
     <t>SMA RA JACK, PCB</t>
   </si>
   <si>
@@ -123,12 +117,6 @@
     <t>CMP-04764-000017-1</t>
   </si>
   <si>
-    <t>149K ohm</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
@@ -189,9 +177,6 @@
     <t>CMP-0136-00723-1</t>
   </si>
   <si>
-    <t>SN74LV1T34DBVR</t>
-  </si>
-  <si>
     <t>IC BUF NON-INVERT 5.5V SOT23-5</t>
   </si>
   <si>
@@ -217,16 +202,101 @@
   </si>
   <si>
     <t>CMP-05700-000010-1</t>
+  </si>
+  <si>
+    <t>Qnty Per Board</t>
+  </si>
+  <si>
+    <t>Link to Part</t>
+  </si>
+  <si>
+    <t>Qnty to Order</t>
+  </si>
+  <si>
+    <t>Indiv Price</t>
+  </si>
+  <si>
+    <t>Total Price</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/kemet/T491X476K035AT/818681</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/kemet/C0805C104J5RAC7025/12701174</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/liteon/LTST-C193KRKT-5A/2356244</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/cui-devices/PJ-063AH/2161208?s=N4IgTCBcDaIAoCkC0AGAbAZgIIAkQF0BfIA</t>
+  </si>
+  <si>
+    <t>733910083</t>
+  </si>
+  <si>
+    <t>0805 Resistor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/molex/0733910083/9740783</t>
+  </si>
+  <si>
+    <t>147K ohm</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/vishay-dale/CRCW0805147KFKEA/1175882</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/RC0805FR-0712KL/727568</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RNCP0805FTD1K00/2240229</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/te-connectivity-passive-product/CRGCQ0805F33R/8576333</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/microchip-technology/MCP1801T-3302I-OT/1679136?s=N4IgTCBcDaILIGEAKBGAHABhQFQLQGZ8MwBJAegHlsQBdAXyA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/microchip-technology/MCP1801T-1802I-OT/1679133?s=N4IgTCBcDaILIGEAKBGAHABhQFQLTozAEkB6AeWxAF0BfIA</t>
+  </si>
+  <si>
+    <t>74LV1T34GV-Q100H</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/analog-devices-inc-maxim-integrated/MAX49140AXK-V/13145155</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/nexperia-usa-inc/74LV1T34GV-Q100H/12337200?s=N4IgTCBcDaIOwBYAyA1AjAFQMwIOIoFoBFNABlIAkQBdAXyA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -270,17 +340,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -593,16 +671,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3E9C9D-9821-4050-91AD-47C3CB425E73}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="18.81640625" customWidth="1"/>
+    <col min="1" max="6" width="18.83203125" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -619,271 +703,445 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="1">
+        <v>10</v>
+      </c>
+      <c r="I2" s="6">
+        <v>2.3279999999999998</v>
+      </c>
+      <c r="J2" s="6">
+        <v>23.28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="F3" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="1">
+        <v>100</v>
+      </c>
+      <c r="I3" s="7">
+        <v>6.13E-2</v>
+      </c>
+      <c r="J3" s="6">
+        <v>6.13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="1">
+        <v>10</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="J4" s="7">
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" s="8">
+        <v>25</v>
+      </c>
+      <c r="I5" s="7">
+        <v>1.274</v>
+      </c>
+      <c r="J5" s="6">
+        <v>31.85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="F6" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="8">
+        <v>25</v>
+      </c>
+      <c r="I6" s="1">
+        <v>4.9829999999999997</v>
+      </c>
+      <c r="J6" s="6">
+        <v>124.58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" s="8">
+        <v>10</v>
+      </c>
+      <c r="I7" s="7">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8" s="8">
+        <v>10</v>
+      </c>
+      <c r="I8" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" s="8">
+        <v>10</v>
+      </c>
+      <c r="I9" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J9" s="6">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="F10" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" s="8">
+        <v>50</v>
+      </c>
+      <c r="I10" s="6">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="J10" s="6">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="8">
+        <v>25</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0.48</v>
+      </c>
+      <c r="J11" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="F12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H12" s="8">
+        <v>25</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0.48</v>
+      </c>
+      <c r="J12" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G13" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H13" s="8">
+        <v>10</v>
+      </c>
+      <c r="I13" s="6">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="J13" s="6">
+        <v>3.82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>
       </c>
+      <c r="G14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="8">
+        <v>10</v>
+      </c>
+      <c r="I14" s="7">
+        <v>2.62</v>
+      </c>
+      <c r="J14" s="6">
+        <v>26.2</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{DA7DE921-1B75-7C45-8D41-C00802C1DE08}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <ignoredErrors>
+    <ignoredError sqref="A6" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed part of level Shifter
Previous part was out of stock so updated level shifter to a similar part
</commit_message>
<xml_diff>
--- a/AnalogComparator/Project Outputs for AnalogComparator/BOM/Bill of Materials-AnalogComparator.xlsx
+++ b/AnalogComparator/Project Outputs for AnalogComparator/BOM/Bill of Materials-AnalogComparator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naomi_12/AnalogComparator/AnalogComparator/Project Outputs for AnalogComparator/BOM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\AnalogComparator\Project Outputs for AnalogComparator\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B512FB0-39B3-104B-ACAF-25285ECB82D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD03F8AA-06CD-4977-AA96-4245A20D73DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-300" yWindow="2120" windowWidth="23200" windowHeight="10020" xr2:uid="{472F2DBD-E0F5-4488-8DC5-87C56A307CF0}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="19200" windowHeight="10010" xr2:uid="{472F2DBD-E0F5-4488-8DC5-87C56A307CF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-AnalogCompara" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="63">
   <si>
     <t>Comment</t>
   </si>
@@ -45,6 +45,9 @@
     <t>LibRef</t>
   </si>
   <si>
+    <t>Quantity</t>
+  </si>
+  <si>
     <t>47uF</t>
   </si>
   <si>
@@ -105,6 +108,9 @@
     <t>CMP-2000-06898-1</t>
   </si>
   <si>
+    <t>73391-0083</t>
+  </si>
+  <si>
     <t>SMA RA JACK, PCB</t>
   </si>
   <si>
@@ -117,6 +123,12 @@
     <t>CMP-04764-000017-1</t>
   </si>
   <si>
+    <t>149K ohm</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>R1</t>
   </si>
   <si>
@@ -177,6 +189,9 @@
     <t>CMP-0136-00723-1</t>
   </si>
   <si>
+    <t>SN74LV1T34DBVR</t>
+  </si>
+  <si>
     <t>IC BUF NON-INVERT 5.5V SOT23-5</t>
   </si>
   <si>
@@ -202,101 +217,16 @@
   </si>
   <si>
     <t>CMP-05700-000010-1</t>
-  </si>
-  <si>
-    <t>Qnty Per Board</t>
-  </si>
-  <si>
-    <t>Link to Part</t>
-  </si>
-  <si>
-    <t>Qnty to Order</t>
-  </si>
-  <si>
-    <t>Indiv Price</t>
-  </si>
-  <si>
-    <t>Total Price</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/kemet/T491X476K035AT/818681</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/kemet/C0805C104J5RAC7025/12701174</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/liteon/LTST-C193KRKT-5A/2356244</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/cui-devices/PJ-063AH/2161208?s=N4IgTCBcDaIAoCkC0AGAbAZgIIAkQF0BfIA</t>
-  </si>
-  <si>
-    <t>733910083</t>
-  </si>
-  <si>
-    <t>0805 Resistor</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/molex/0733910083/9740783</t>
-  </si>
-  <si>
-    <t>147K ohm</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/vishay-dale/CRCW0805147KFKEA/1175882</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/yageo/RC0805FR-0712KL/727568</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RNCP0805FTD1K00/2240229</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/te-connectivity-passive-product/CRGCQ0805F33R/8576333</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/microchip-technology/MCP1801T-3302I-OT/1679136?s=N4IgTCBcDaILIGEAKBGAHABhQFQLQGZ8MwBJAegHlsQBdAXyA</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/microchip-technology/MCP1801T-1802I-OT/1679133?s=N4IgTCBcDaILIGEAKBGAHABhQFQLTozAEkB6AeWxAF0BfIA</t>
-  </si>
-  <si>
-    <t>74LV1T34GV-Q100H</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/analog-devices-inc-maxim-integrated/MAX49140AXK-V/13145155</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/nexperia-usa-inc/74LV1T34GV-Q100H/12337200?s=N4IgTCBcDaIOwBYAyA1AjAFQMwIOIoFoBFNABlIAkQBdAXyA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0.00"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -340,25 +270,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -671,22 +593,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3E9C9D-9821-4050-91AD-47C3CB425E73}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="6" width="18.83203125" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" customWidth="1"/>
-    <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="15.5" customWidth="1"/>
+    <col min="1" max="6" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -703,445 +619,271 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H2" s="1">
-        <v>10</v>
-      </c>
-      <c r="I2" s="6">
-        <v>2.3279999999999998</v>
-      </c>
-      <c r="J2" s="6">
-        <v>23.28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" s="1">
         <v>5</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H3" s="1">
-        <v>100</v>
-      </c>
-      <c r="I3" s="7">
-        <v>6.13E-2</v>
-      </c>
-      <c r="J3" s="6">
-        <v>6.13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H4" s="1">
-        <v>10</v>
-      </c>
-      <c r="I4" s="7">
-        <v>0.21099999999999999</v>
-      </c>
-      <c r="J4" s="7">
-        <v>2.11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H5" s="8">
-        <v>25</v>
-      </c>
-      <c r="I5" s="7">
-        <v>1.274</v>
-      </c>
-      <c r="J5" s="6">
-        <v>31.85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F6" s="1">
         <v>2</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H6" s="8">
-        <v>25</v>
-      </c>
-      <c r="I6" s="1">
-        <v>4.9829999999999997</v>
-      </c>
-      <c r="J6" s="6">
-        <v>124.58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H7" s="8">
-        <v>10</v>
-      </c>
-      <c r="I7" s="7">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="J7" s="6">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H8" s="8">
-        <v>10</v>
-      </c>
-      <c r="I8" s="7">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="J8" s="6">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="F9" s="1">
         <v>1</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H9" s="8">
-        <v>10</v>
-      </c>
-      <c r="I9" s="10">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="J9" s="6">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F10" s="1">
         <v>2</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H10" s="8">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I10" s="6">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="J10" s="6">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H11" s="8">
-        <v>25</v>
-      </c>
-      <c r="I11" s="6">
-        <v>0.48</v>
-      </c>
-      <c r="J11" s="6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="C12" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F12" s="1">
         <v>1</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H12" s="8">
-        <v>25</v>
-      </c>
-      <c r="I12" s="6">
-        <v>0.48</v>
-      </c>
-      <c r="J12" s="6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
       </c>
-      <c r="G13" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H13" s="8">
-        <v>10</v>
-      </c>
-      <c r="I13" s="6">
-        <v>0.38200000000000001</v>
-      </c>
-      <c r="J13" s="6">
-        <v>3.82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H14" s="8">
-        <v>10</v>
-      </c>
-      <c r="I14" s="7">
-        <v>2.62</v>
-      </c>
-      <c r="J14" s="6">
-        <v>26.2</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{DA7DE921-1B75-7C45-8D41-C00802C1DE08}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <ignoredErrors>
-    <ignoredError sqref="A6" numberStoredAsText="1"/>
-  </ignoredErrors>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated BOM with new level shifter part
</commit_message>
<xml_diff>
--- a/AnalogComparator/Project Outputs for AnalogComparator/BOM/Bill of Materials-AnalogComparator.xlsx
+++ b/AnalogComparator/Project Outputs for AnalogComparator/BOM/Bill of Materials-AnalogComparator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naomi_12/AnalogComparator/AnalogComparator/Project Outputs for AnalogComparator/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B512FB0-39B3-104B-ACAF-25285ECB82D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7F3BA8-E503-8343-9C9D-2F633884B0E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-300" yWindow="2120" windowWidth="23200" windowHeight="10020" xr2:uid="{472F2DBD-E0F5-4488-8DC5-87C56A307CF0}"/>
+    <workbookView xWindow="0" yWindow="2120" windowWidth="23200" windowHeight="10020" xr2:uid="{472F2DBD-E0F5-4488-8DC5-87C56A307CF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-AnalogCompara" sheetId="1" r:id="rId1"/>
@@ -276,7 +276,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -344,7 +344,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -352,10 +352,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -674,7 +673,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -836,7 +835,7 @@
       <c r="G5" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="1">
         <v>25</v>
       </c>
       <c r="I5" s="7">
@@ -868,7 +867,7 @@
       <c r="G6" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="1">
         <v>25</v>
       </c>
       <c r="I6" s="1">
@@ -900,7 +899,7 @@
       <c r="G7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="1">
         <v>10</v>
       </c>
       <c r="I7" s="7">
@@ -932,7 +931,7 @@
       <c r="G8" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="1">
         <v>10</v>
       </c>
       <c r="I8" s="7">
@@ -964,10 +963,10 @@
       <c r="G9" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="1">
         <v>10</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="7">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="J9" s="6">
@@ -996,7 +995,7 @@
       <c r="G10" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="1">
         <v>50</v>
       </c>
       <c r="I10" s="6">
@@ -1028,7 +1027,7 @@
       <c r="G11" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="1">
         <v>25</v>
       </c>
       <c r="I11" s="6">
@@ -1057,10 +1056,10 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="1">
         <v>25</v>
       </c>
       <c r="I12" s="6">
@@ -1092,7 +1091,7 @@
       <c r="G13" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="1">
         <v>10</v>
       </c>
       <c r="I13" s="6">
@@ -1124,7 +1123,7 @@
       <c r="G14" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="1">
         <v>10</v>
       </c>
       <c r="I14" s="7">
@@ -1137,9 +1136,11 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{DA7DE921-1B75-7C45-8D41-C00802C1DE08}"/>
+    <hyperlink ref="G12" r:id="rId2" xr:uid="{35D01929-7467-8C4E-BF8A-C1C39EDF0E38}"/>
+    <hyperlink ref="G13" r:id="rId3" xr:uid="{8C084D8F-3665-2841-85FF-A92451EAF3F1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
   <ignoredErrors>
     <ignoredError sqref="A6" numberStoredAsText="1"/>
   </ignoredErrors>

</xml_diff>